<commit_message>
Version sin errores, falta correguir posibles fallos de internet
</commit_message>
<xml_diff>
--- a/output/main/testBaseDeDatos.xlsx
+++ b/output/main/testBaseDeDatos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Esteban\OneDrive - Universidad Sergio Arboleda\Escritorio\PythonSelenium\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas Esteban\Escritorio\PythonSelenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B342C806-2850-4FCD-86FE-906AC34E7F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4598F1B-36B0-4068-B217-A3E28D675946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6476DFB1-9FF7-436A-B759-4FD0DD3C30F3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="917">
   <si>
     <t>NUMERO DEL PROCESO</t>
   </si>
@@ -3685,7 +3685,7 @@
   <dimension ref="A1:D1228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3721,7 +3721,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3735,7 +3735,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3752,9 +3752,6 @@
       </c>
       <c r="B5">
         <v>456456456</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4">

</xml_diff>